<commit_message>
modified classes is added
</commit_message>
<xml_diff>
--- a/testng_project/src/test/resources/TestData/KeywordDriven.xlsx
+++ b/testng_project/src/test/resources/TestData/KeywordDriven.xlsx
@@ -31,7 +31,7 @@
     <t>pages.Logout</t>
   </si>
   <si>
-    <t>tc01</t>
+    <t>testCase01</t>
   </si>
   <si>
     <t>openBrowser</t>
@@ -47,6 +47,24 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>testCase02</t>
+  </si>
+  <si>
+    <t>testCase03</t>
+  </si>
+  <si>
+    <t>testCase04</t>
+  </si>
+  <si>
+    <t>testCase05</t>
+  </si>
+  <si>
+    <t>testCase06</t>
+  </si>
+  <si>
+    <t>testCase07</t>
   </si>
 </sst>
 </file>
@@ -377,7 +395,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,6 +448,108 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>